<commit_message>
More small changes to plotting and file names
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_221026.xlsx
+++ b/data/hake_intrasp_221026.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F176F54D-CCFB-4F49-A104-4F67111ABD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784ABFC4-CC6F-2A45-A34A-96F40BC79EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="500" windowWidth="38400" windowHeight="33340" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -11705,8 +11705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:V1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11817,49 +11817,49 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="D2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="E2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="F2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="G2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="H2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="I2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="J2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="K2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="L2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="M2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="N2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="O2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="P2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
       <c r="Q2">
-        <v>0.214</v>
+        <v>0.21</v>
       </c>
     </row>
   </sheetData>
@@ -17194,7 +17194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>

</xml_diff>